<commit_message>
Carga del administrador de Catalogos.
Funcionalidad de control de catalogos.
</commit_message>
<xml_diff>
--- a/Documentacion/Miselaneos/ErroresDelSistema.xlsx
+++ b/Documentacion/Miselaneos/ErroresDelSistema.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BC961C-5F0D-417C-832E-6C67E73184EE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0945682-F097-42D1-9D2B-E8E460708E63}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Errores" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="72">
   <si>
     <t>El sistema no pudo encontrar el registro solicitado o la conexión no está disponible. Contacte con su administrador.</t>
   </si>
@@ -201,6 +206,45 @@
   </si>
   <si>
     <t>La contraseña no cumple con las politicas definidas o la confirmacion fallo. Por favor valide e intente de nuevo.</t>
+  </si>
+  <si>
+    <t>Para que el cambio tenga efecto deberá reiniciar su sesión.</t>
+  </si>
+  <si>
+    <t>Se ha presentado un problema al modificar el catálogo. Intente nuevamente. Si el problema persiste contacte con su administrador</t>
+  </si>
+  <si>
+    <t>Error al modificar el catálogo</t>
+  </si>
+  <si>
+    <t>Éxito al modificar el catálogo</t>
+  </si>
+  <si>
+    <t>Se a actualizado correctamente el catálogo</t>
+  </si>
+  <si>
+    <t>El catálogo $ ha sido guardado correctamente, junto con el item $.</t>
+  </si>
+  <si>
+    <t>Éxito al crear el catálogo</t>
+  </si>
+  <si>
+    <t>El catálogo $ no ha sido guardado correctamente, junto con el item $. Si el problema perisite contacte con su administrador</t>
+  </si>
+  <si>
+    <t>Error al crear el catálogo</t>
+  </si>
+  <si>
+    <t>Ha ocurrido un error inesperado al guardar el catálogo. Si el problema persiste contacte con su administrador</t>
+  </si>
+  <si>
+    <t>FATAL</t>
+  </si>
+  <si>
+    <t>Se ha presentado un error al tratar de recuperar los catálogos actuales. Si el problema persiste contacte con su administrador</t>
+  </si>
+  <si>
+    <t>Error al recuperar la vista</t>
   </si>
 </sst>
 </file>
@@ -541,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,6 +1931,15 @@
       <c r="B36">
         <v>35</v>
       </c>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" t="s">
+        <v>62</v>
+      </c>
       <c r="F36" t="str">
         <f t="shared" si="6"/>
         <v>SYSTEM</v>
@@ -1917,6 +1970,15 @@
       <c r="B37">
         <v>36</v>
       </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" t="s">
+        <v>62</v>
+      </c>
       <c r="F37" t="str">
         <f t="shared" si="6"/>
         <v>SYSTEM</v>
@@ -1946,6 +2008,15 @@
       <c r="B38">
         <v>37</v>
       </c>
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>61</v>
+      </c>
       <c r="F38" t="str">
         <f t="shared" si="6"/>
         <v>SYSTEM</v>
@@ -1975,6 +2046,15 @@
       <c r="B39">
         <v>38</v>
       </c>
+      <c r="C39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" t="s">
+        <v>65</v>
+      </c>
       <c r="F39" t="str">
         <f t="shared" si="6"/>
         <v>SYSTEM</v>
@@ -2004,6 +2084,15 @@
       <c r="B40">
         <v>39</v>
       </c>
+      <c r="C40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>67</v>
+      </c>
       <c r="F40" t="str">
         <f t="shared" si="6"/>
         <v>SYSTEM</v>
@@ -2033,6 +2122,15 @@
       <c r="B41">
         <v>40</v>
       </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" t="s">
+        <v>67</v>
+      </c>
       <c r="F41" t="str">
         <f t="shared" si="6"/>
         <v>SYSTEM</v>
@@ -2062,6 +2160,15 @@
       <c r="B42">
         <v>41</v>
       </c>
+      <c r="C42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" t="s">
+        <v>71</v>
+      </c>
       <c r="F42" t="str">
         <f t="shared" si="6"/>
         <v>SYSTEM</v>
@@ -2091,6 +2198,7 @@
       <c r="B43">
         <v>42</v>
       </c>
+      <c r="E43" s="5"/>
       <c r="F43" t="str">
         <f t="shared" si="6"/>
         <v>SYSTEM</v>
@@ -6071,8 +6179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F02A1FF-E39E-464F-B66C-DC6E14088AF1}">
   <dimension ref="B2:B166"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B34" sqref="B32:B34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6284,43 +6392,43 @@
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>CONCATENATE("INSERT INTO AD_ERROR VALUES (",Errores!B36,", '",Errores!C36,"', '",Errores!D36,"', '",Errores!E36,"', '",Errores!F36,"', '",Errores!G36,"', ",Errores!H36,",",Errores!I36,",",Errores!J36,",",Errores!K36,");")</f>
-        <v>INSERT INTO AD_ERROR VALUES (35, '', '', '', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
+        <v>INSERT INTO AD_ERROR VALUES (35, 'Se a actualizado correctamente el catálogo', 'INFO', 'Éxito al modificar el catálogo', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>CONCATENATE("INSERT INTO AD_ERROR VALUES (",Errores!B37,", '",Errores!C37,"', '",Errores!D37,"', '",Errores!E37,"', '",Errores!F37,"', '",Errores!G37,"', ",Errores!H37,",",Errores!I37,",",Errores!J37,",",Errores!K37,");")</f>
-        <v>INSERT INTO AD_ERROR VALUES (36, '', '', '', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
+        <v>INSERT INTO AD_ERROR VALUES (36, 'Para que el cambio tenga efecto deberá reiniciar su sesión.', 'WARN', 'Éxito al modificar el catálogo', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>CONCATENATE("INSERT INTO AD_ERROR VALUES (",Errores!B38,", '",Errores!C38,"', '",Errores!D38,"', '",Errores!E38,"', '",Errores!F38,"', '",Errores!G38,"', ",Errores!H38,",",Errores!I38,",",Errores!J38,",",Errores!K38,");")</f>
-        <v>INSERT INTO AD_ERROR VALUES (37, '', '', '', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
+        <v>INSERT INTO AD_ERROR VALUES (37, 'Se ha presentado un problema al modificar el catálogo. Intente nuevamente. Si el problema persiste contacte con su administrador', 'ERROR', 'Error al modificar el catálogo', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>CONCATENATE("INSERT INTO AD_ERROR VALUES (",Errores!B39,", '",Errores!C39,"', '",Errores!D39,"', '",Errores!E39,"', '",Errores!F39,"', '",Errores!G39,"', ",Errores!H39,",",Errores!I39,",",Errores!J39,",",Errores!K39,");")</f>
-        <v>INSERT INTO AD_ERROR VALUES (38, '', '', '', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
+        <v>INSERT INTO AD_ERROR VALUES (38, 'El catálogo $ ha sido guardado correctamente, junto con el item $.', 'INFO', 'Éxito al crear el catálogo', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>CONCATENATE("INSERT INTO AD_ERROR VALUES (",Errores!B40,", '",Errores!C40,"', '",Errores!D40,"', '",Errores!E40,"', '",Errores!F40,"', '",Errores!G40,"', ",Errores!H40,",",Errores!I40,",",Errores!J40,",",Errores!K40,");")</f>
-        <v>INSERT INTO AD_ERROR VALUES (39, '', '', '', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
+        <v>INSERT INTO AD_ERROR VALUES (39, 'El catálogo $ no ha sido guardado correctamente, junto con el item $. Si el problema perisite contacte con su administrador', 'ERROR', 'Error al crear el catálogo', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>CONCATENATE("INSERT INTO AD_ERROR VALUES (",Errores!B41,", '",Errores!C41,"', '",Errores!D41,"', '",Errores!E41,"', '",Errores!F41,"', '",Errores!G41,"', ",Errores!H41,",",Errores!I41,",",Errores!J41,",",Errores!K41,");")</f>
-        <v>INSERT INTO AD_ERROR VALUES (40, '', '', '', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
+        <v>INSERT INTO AD_ERROR VALUES (40, 'Ha ocurrido un error inesperado al guardar el catálogo. Si el problema persiste contacte con su administrador', 'FATAL', 'Error al crear el catálogo', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>CONCATENATE("INSERT INTO AD_ERROR VALUES (",Errores!B42,", '",Errores!C42,"', '",Errores!D42,"', '",Errores!E42,"', '",Errores!F42,"', '",Errores!G42,"', ",Errores!H42,",",Errores!I42,",",Errores!J42,",",Errores!K42,");")</f>
-        <v>INSERT INTO AD_ERROR VALUES (41, '', '', '', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
+        <v>INSERT INTO AD_ERROR VALUES (41, 'Se ha presentado un error al tratar de recuperar los catálogos actuales. Si el problema persiste contacte con su administrador', 'FATAL', 'Error al recuperar la vista', 'SYSTEM', 'SYSTEM', to_timestamp(sysdate,'DD/MM/RR HH12:MI:SSXFF AM'),1,to_date(sysdate,'DD/MM/RR'),0);</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>